<commit_message>
In progress gradient subgraph.
</commit_message>
<xml_diff>
--- a/spinnaker_graph_front_end/examples/TensorSample/GradientAnalysis.xlsx
+++ b/spinnaker_graph_front_end/examples/TensorSample/GradientAnalysis.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Documents\spinnaker\SpiNNakerGraphFrontEnd\spinnaker_graph_front_end\examples\TensorSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BC42A1-2A57-4F58-9F09-0CE2ACCE6BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0E5763-F3FD-4752-902B-A8C4523ABB7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="240" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{DE7DD880-2A49-478E-9D36-1329DA80DE3F}"/>
+    <workbookView xWindow="16665" yWindow="6660" windowWidth="13170" windowHeight="9255" activeTab="2" xr2:uid="{DE7DD880-2A49-478E-9D36-1329DA80DE3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Gradient Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Operations" sheetId="2" r:id="rId2"/>
+    <sheet name="Const Values" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Gradient Inputs</t>
   </si>
@@ -202,13 +203,155 @@
   </si>
   <si>
     <t>gradients/Log_grad/mul 2x10</t>
+  </si>
+  <si>
+    <t>gradients/Log_grad/Reciprocal 1x10
+gradients/mul_grad/tuple/control_dependency 1x10</t>
+  </si>
+  <si>
+    <t>gradients/Softmax_grad/mul 1x10
+gradients/Softmax_grad/sub 1x10</t>
+  </si>
+  <si>
+    <t>Softmax_gr</t>
+  </si>
+  <si>
+    <t>Const Values</t>
+  </si>
+  <si>
+    <t>gradients/Shape</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>gradients/grad_ys_0</t>
+  </si>
+  <si>
+    <t>Op</t>
+  </si>
+  <si>
+    <t>Neg</t>
+  </si>
+  <si>
+    <t>gradients/Sum_grad/Reshape/shape</t>
+  </si>
+  <si>
+    <t>Const</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>gradients/Sum_grad/Const</t>
+  </si>
+  <si>
+    <t>[1 10]</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Here just set the shape 1 1 which is actual a shape of a scalar, no practical change.</t>
+  </si>
+  <si>
+    <t>1 float</t>
+  </si>
+  <si>
+    <t>This operation creates a tensor of shape dims and fills it with value</t>
+  </si>
+  <si>
+    <t>Computes numerical negative value element-wise.</t>
+  </si>
+  <si>
+    <r>
+      <t>Given </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF37474F"/>
+        <rFont val="Roboto Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>tensor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Noto Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>, this operation returns a tensor that has the same values as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF37474F"/>
+        <rFont val="Roboto Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>tensor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Noto Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t> with shape </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF37474F"/>
+        <rFont val="Roboto Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>shape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Noto Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>is the input to tile</t>
+  </si>
+  <si>
+    <t>gradients/Sum_grad/Tile</t>
+  </si>
+  <si>
+    <t>return a tensor 1x10</t>
+  </si>
+  <si>
+    <t>gradients/mul_grad/Mul</t>
+  </si>
+  <si>
+    <t>multiplies log and tile</t>
+  </si>
+  <si>
+    <t>gradients/mul_grad/Mul1</t>
+  </si>
+  <si>
+    <t>multiplies placeholder and tile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +359,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF202124"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF37474F"/>
+      <name val="Roboto Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +392,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -240,17 +407,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,17 +742,17 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" customWidth="1"/>
     <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.81640625" customWidth="1"/>
     <col min="7" max="7" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -616,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -636,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -656,7 +829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -664,7 +837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -679,21 +852,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C45D6EA-4E67-4264-A622-1B80FFCD1807}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.1796875" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -710,7 +883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -727,7 +900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -741,12 +914,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -760,7 +933,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -774,12 +947,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -790,7 +963,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -801,12 +974,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -815,9 +988,156 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F36C6E-0D53-4EDD-8C35-EBD1AE3B0733}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="144" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>